<commit_message>
Save 19 08 2025
</commit_message>
<xml_diff>
--- a/4 четверть_9_JavaScript_Vue.xlsx
+++ b/4 четверть_9_JavaScript_Vue.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6CABF9-5989-4A9A-B8C3-F8668DDF3B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0668566-853F-44AB-BB49-F3BEBF1B9B8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Название 1-3" sheetId="12" r:id="rId1"/>
     <sheet name="Vuetify" sheetId="15" r:id="rId2"/>
     <sheet name="snippets Vue" sheetId="14" r:id="rId3"/>
+    <sheet name="download CSV" sheetId="16" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="466">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -7016,6 +7017,192 @@
         <scheme val="minor"/>
       </rPr>
       <t>vp</t>
+    </r>
+  </si>
+  <si>
+    <t>CSV downloader</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">import Vue from 'vue';
+import { mapState, mapGetters } from 'vuex';
+import template from './ApiViewPfields.html';
+import { createObjectCsvStringifier } from 'csv-writer-browser';
+export default Vue.extend({
+    template,
+    name: 'ApiViewPfields',
+    components: {
+    },
+    data(){
+        return {
+            loading_state: false,
+            table: null,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            csvHeaders: [
+                    {id: 'FieldNameRu', title: 'FieldNameRu'},
+                    {id: 'FieldNm', title: 'FieldNm'},
+                    {id: 'FieldTable', title: 'FieldTable'},
+                    {id: 'FieldType', title: 'FieldType'},
+                    {id: 'NoValid', title: 'NoValid'},
+                    {id: 'RelatedCatalog', title: 'RelatedCatalog'},
+                    {id: 'RelatedCatalogKey', title: 'RelatedCatalogKey'},
+                    {id: 'StorageProcedure', title: 'StorageProcedure'},
+                    {id: 'Comment', title: 'Comment'},
+                    {id: 'SYSDATE', title: 'SYSDATE'},
+                ],
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        }
+    },</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    mounted(){
+        this.getApiViewPfields();
+    },
+    computed: {
+        ...mapState({
+            loading: state =&gt; state.user.loading
+        }),
+        fieldNames: function() {
+            return Object.keys(this.table[0]);
+        },
+    },
+    methods: {
+        async getApiViewPfields() {
+            this.loading_state = true;
+            this.$http.post('/api/manage/getApiViewPfields')
+                .then((res) =&gt; {
+                    this.table = res.body;
+                    console.log(this.table);
+                })                  
+                .finally(() =&gt; {
+                    this.loading_state = false
+                });
+        },</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        getCsv(){
+            const csvStringifier = createObjectCsvStringifier({
+              header: this.csvHeaders
+            }); 
+            const csvHeader = csvStringifier.getHeaderString();
+            const csvBody = csvStringifier.stringifyRecords(this.table);
+            const csvContent = "\uFEFF" + csvHeader + csvBody;
+            const blob = new Blob([csvContent], { type: 'text/csv;charset=utf-8;'});
+            const url = URL.createObjectURL(blob);  
+            const link = document.createElement('a');
+            link.setAttribute('href', url);
+            link.setAttribute('download', 'my_data.csv');
+            document.body.appendChild(link);
+            link.click();
+            document.body.removeChild(link);
+            URL.revokeObjectURL(url);
+        }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+    }
+});</t>
+    </r>
+  </si>
+  <si>
+    <t>CSV downloader.js</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;div 
+    style="margin: 0px 36px"
+&gt;
+&lt;div&gt;
+    &lt;el-table
+        :data="table"
+        :default-sort = "{prop: 'FieldNameRu', order: 'descending'}"
+        style=
+        "
+        height: 80vh; 
+        overflow-y: auto;
+        text-align: left; "
+        &gt;
+        &lt;el-table-column
+            v-for="(item, index) in fieldNames"
+            :key="`${item}-${index}`"
+            :prop="item"
+            :label="$t(`${item}`)"
+            :sortable="item === `FieldNameRu` || item === `StorageProcedure`"&gt;
+        &lt;/el-table-column&gt;
+  &lt;/el-table&gt;
+&lt;/div&gt;
+    &lt;div style="margin-top: 24px; display: flex; justify-content: center;"&gt;
+        &lt;a class="btn btn-default hwc-btn-unactive" style="width:25vw" v-on:click="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>getCsv()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;
+            CSV
+        &lt;/a&gt;
+    &lt;/div&gt;
+&lt;/div&gt;</t>
     </r>
   </si>
 </sst>
@@ -7404,7 +7591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -7554,6 +7741,15 @@
     </xf>
     <xf numFmtId="49" fontId="12" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -8633,7 +8829,7 @@
   </sheetPr>
   <dimension ref="A2:V286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -11327,4 +11523,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F33576-E5EF-47DE-AAF9-4DE2FAE178AB}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:V9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="36" style="20" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="22"/>
+    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="U2" s="24"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="C3" s="52" t="s">
+        <v>459</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="21"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="54" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="409.6">
+      <c r="C5" s="53" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="331.2">
+      <c r="C6" s="53" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="273.60000000000002">
+      <c r="C7" s="53" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="54" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="409.6">
+      <c r="C9" s="53" t="s">
+        <v>465</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
save 04 12 2025
</commit_message>
<xml_diff>
--- a/4 четверть_9_JavaScript_Vue.xlsx
+++ b/4 четверть_9_JavaScript_Vue.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23800E79-1B6A-4505-AA46-6DBEDC3E44F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D310908-9A55-4616-8654-437D3C04E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Название 1-3" sheetId="12" r:id="rId1"/>
     <sheet name="Vue Css" sheetId="17" r:id="rId2"/>
-    <sheet name="ElComponent" sheetId="18" r:id="rId3"/>
-    <sheet name="El-dialog" sheetId="19" r:id="rId4"/>
-    <sheet name="Vuetify" sheetId="15" r:id="rId5"/>
-    <sheet name="snippets Vue" sheetId="14" r:id="rId6"/>
-    <sheet name="download CSV" sheetId="16" r:id="rId7"/>
+    <sheet name="URL to login after REMOTE auth" sheetId="20" r:id="rId3"/>
+    <sheet name="ElComponent" sheetId="18" r:id="rId4"/>
+    <sheet name="El-dialog" sheetId="19" r:id="rId5"/>
+    <sheet name="Vuetify" sheetId="15" r:id="rId6"/>
+    <sheet name="snippets Vue" sheetId="14" r:id="rId7"/>
+    <sheet name="download CSV" sheetId="16" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="485">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="494">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -7636,17 +7637,170 @@
   <si>
     <t>El-dialog</t>
   </si>
+  <si>
+    <t>Вход в SPA после авторизации на стороннем сайте</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      loginWithJwtFromAnotherWebsite(){
+        let jwt = this.$route.query.jwt;
+        this.$http.post('/api/auth/getUserData', {access_token:jwt})
+          .then(response =&gt; {
+            asyncLocalStorageLk.setItem('token', JSON.stringify(response.data))
+        	    .then(() =&gt; {
+        	    	Store.commit('user/setToken', {access_token:jwt});
+        	    	this.getHttpDict();
+        	    	this.getUserData();
+        	    	this.$router.push('/');
+        	  });
+          })
+          .catch(err =&gt; {
+            console.log(`Ответ: ${err}`);
+          });
+      },</t>
+  </si>
+  <si>
+    <t>methods:</t>
+  </si>
+  <si>
+    <t>beforeMount(){}</t>
+  </si>
+  <si>
+    <t>if(this.$route.name === 'loginsite') this.loginWithJwtFromAnotherWebsite();</t>
+  </si>
+  <si>
+    <t>routes.js</t>
+  </si>
+  <si>
+    <t>const routes = [
+  {
+    path: '/',
+    name: 'home',
+    component: () =&gt; import ('src/components/Home/home'),//Home,
+    panel: 'Рабочая панель'
+  },
+  // {
+  //   path: '/analitic/:path',
+  //   name: 'Analitic',
+  //   component: () =&gt; import ('src/components/Analitic/Analitic'),//Analitic,
+  //   panel: 'Аналитика'
+  // },
+  {
+    path: '/base/:path',
+    name: 'base',
+    component: () =&gt; import ('src/components/Bases/Bases'),//Bases,
+    panel: 'Базы'
+  },
+  {
+    path: '/manual',
+    name: 'manual',
+    component: () =&gt; import ('src/components/Manage/Help/Help'),//Help,
+    panel: 'Помощь'
+  },
+  {
+    path: '/manual/:dict',
+    name: 'manual',
+    component: () =&gt; import ('src/components/Manage/Help/Help'),//Help,
+    panel: 'Помощь'
+  },
+  {
+    path: '/calendar/:path',
+    name: 'calendar',
+    component: () =&gt; import ('src/components/Calendar/Calendar'),//Calendar,
+    panel: 'Календарь'
+  },
+  {
+    path: '/journal',
+    name: 'journal',
+    component: () =&gt; import ('src/components/Journal/Journal'),//Journal,
+    panel: 'Журнал'
+  },
+  {
+    path: '/manage/:path',
+    name: 'manage',
+    component: () =&gt; import ('src/components/Manage/Manage'),//Manage,
+    panel: 'Управление'
+  },
+  {
+    path: '/manage/:path/app/:appid',
+    name: 'manage',
+    component: () =&gt; import ('src/components/Manage/Manage'),//Manage,
+    panel: 'Управление'
+  },
+  {
+    path: '/profile',
+    name: 'profile',
+    component: () =&gt; import ('src/components/Profile/profile'),//Profile
+  },
+  {
+    path: '/files',
+    name: 'files',
+    component: () =&gt; import ('src/components/Files/Files'),//Files
+  },
+  {
+    path: '/hwcbi',
+    name: 'hwcbi',
+    component: () =&gt; import ('src/components/HWCBI/HWCBI.js'),//Files
+  },
+  {
+    path: '/lined/:base/:id',
+    name: 'linedview',
+    component: () =&gt; import ('src/components/LinedView/LinedView'),//LinedView
+  },
+  {
+    path: '/linedanalitic/:id',
+    name: 'linedanalitic',
+    component: () =&gt; import ('src/components/LinedAnalitic/LinedAnalitic'),//LinedAnalitic
+  },
+  {
+    path: '/login/:type/:key',
+    name: 'login',
+  },
+  {
+    path: '/loginsite/',
+    name: 'loginsite',
+  },
+  {
+    path: '*',
+    name: 'notfound',
+    component: () =&gt; import ('components/NotFound/notFound'), //NotFound,
+    panel: 'Страница не найдена'
+  }
+];
+export default routes;</t>
+  </si>
+  <si>
+    <t>https://test.hwcompany.ru/loginsite?jwt={$access_token}</t>
+  </si>
+  <si>
+    <t>Результат должен быть</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="37">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -7940,6 +8094,14 @@
       <color rgb="FF213547"/>
       <name val="Var(--vt-font-family-mono)"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -8042,11 +8204,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -8057,20 +8220,20 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -8082,7 +8245,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -8094,60 +8257,69 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8155,7 +8327,7 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -8164,8 +8336,8 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8173,38 +8345,47 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8212,26 +8393,30 @@
     <xf numFmtId="49" fontId="2" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{141A142D-D8A7-43F9-B8D2-54AA311FA1CB}"/>
   </cellStyles>
@@ -11700,7 +11885,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="19" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -11715,8 +11900,8 @@
   </sheetPr>
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -11751,10 +11936,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="23"/>
@@ -11838,6 +12023,169 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D825E87-AA95-4E22-841B-0301C795364F}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:V8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="36" style="20" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
+    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="22"/>
+    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="U2" s="24"/>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="C3" s="61" t="s">
+        <v>485</v>
+      </c>
+      <c r="P3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="21"/>
+    </row>
+    <row r="4" spans="1:22" s="19" customFormat="1">
+      <c r="A4" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="30"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="22"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="20"/>
+    </row>
+    <row r="5" spans="1:22" s="19" customFormat="1">
+      <c r="A5" s="68" t="s">
+        <v>493</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="69" t="s">
+        <v>492</v>
+      </c>
+      <c r="D5" s="30"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="21"/>
+      <c r="V5" s="20"/>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="63" t="s">
+        <v>489</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="230.4">
+      <c r="A7" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="63" t="s">
+        <v>486</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" ht="409.6">
+      <c r="A8" s="64" t="s">
+        <v>490</v>
+      </c>
+      <c r="C8" s="65" t="s">
+        <v>491</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{984FD18E-33B2-4540-A010-FE3C4F5272D7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10679322-B66C-4A2A-BA00-35BB5CDCF52D}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
@@ -11881,10 +12229,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="23"/>
@@ -11906,10 +12254,10 @@
       <c r="U2" s="24"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>468</v>
       </c>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="58" t="s">
         <v>467</v>
       </c>
       <c r="P3" s="20"/>
@@ -11925,7 +12273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB89C57B-4415-4E7B-A67D-1BB77B7555B3}">
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
@@ -11933,7 +12281,7 @@
   </sheetPr>
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -11969,10 +12317,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="23"/>
@@ -11994,74 +12342,74 @@
       <c r="U2" s="24"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>484</v>
       </c>
-      <c r="D3" s="60"/>
+      <c r="D3" s="58"/>
       <c r="P3" s="20"/>
       <c r="U3" s="20"/>
       <c r="V3" s="21"/>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="60" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="129.6">
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="59" t="s">
         <v>471</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="216">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="58" t="s">
         <v>473</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="59" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="316.8">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="58" t="s">
         <v>474</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="59" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="360">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="58" t="s">
         <v>477</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="59" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="331.2">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="58" t="s">
         <v>479</v>
       </c>
-      <c r="C9" s="61" t="s">
+      <c r="C9" s="59" t="s">
         <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="374.4">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="58" t="s">
         <v>478</v>
       </c>
-      <c r="C10" s="61" t="s">
+      <c r="C10" s="59" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="60" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="409.6">
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="59" t="s">
         <v>481</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="59" t="s">
         <v>480</v>
       </c>
     </row>
@@ -12074,7 +12422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA43F35-896E-4AF4-9490-A6E7A4167F76}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12117,10 +12465,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="23"/>
@@ -12227,7 +12575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28329730-A06B-4EF9-BB9C-FF8DE4151289}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12270,12 +12618,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="67" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="23"/>
@@ -12349,7 +12697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F33576-E5EF-47DE-AAF9-4DE2FAE178AB}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12392,10 +12740,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
+      <c r="A1" s="66"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="23"/>

</xml_diff>

<commit_message>
save 13 12 2025
</commit_message>
<xml_diff>
--- a/4 четверть_9_JavaScript_Vue.xlsx
+++ b/4 четверть_9_JavaScript_Vue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Machenike\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D310908-9A55-4616-8654-437D3C04E031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F180E0-0AA0-4CEF-BBBA-ECA73963BA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Название 1-3" sheetId="12" r:id="rId1"/>
@@ -27,15 +27,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="500">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -6897,99 +6894,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">                &lt;el-button
-                    style="
-                        box-sizing: border-box;
-                        width: calc(100% / 3);
-                        margin-right: 0px;
-                        margin-left: 0px;
-                    "
-                    type="button"
-                    size="mini"
-                    class="btn el-filter-icon fa fa-align-justify"
-                   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :style="condformattingobj.colorformatting?.active ? activeStyleColor : {}"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                    v-on:click="addColorFormatting"
-                &gt;
-                &lt;/el-button&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">data() {
-        return {
-            valueTypesDict: {
-                maxbydefault: "Максимальное значение",
-                minbydefault: "Минимальное значение",
-                number: "Число",
-                percent: "Процент",
-                percentile: "Процентиль",
-            },
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">            activeStyleColor: {
-                backgroundColor: "#409EFF",
-                borderColor: "#409EFF",
-                color: "#fff",
-            },
-            activeStyleHistogram: {
-                backgroundColor: "#9C9E21",
-                borderColor: "#9C9E21",
-                color: "#fff",
-            },
-            activeStyleIcon: {
-                backgroundColor: "#AD3131",
-                borderColor: "#AD3131",
-                color: "#fff",
-            },
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">        };
-    },</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">vue create </t>
     </r>
     <r>
@@ -7211,44 +7115,6 @@
   </si>
   <si>
     <t>Vue Css</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                      &lt;button 
-                              class="btn btn-xs panel-btn fa fa-lightbulb-o"
-                              v-bind:class="
-                              {
-                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'btn-danger': colorEdit &amp;&amp; baseSettings.editUserCurrentSetting,
-                                'btn-default': !colorEdit || !baseSettings.editUserCurrentSetting, 
-                                'btn-primary': colorEdit &amp;&amp; !baseSettings.editUserCurrentSetting</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                              }
-                              "
-                              v-on:click="changeEditorToColor"&gt;
-                      &lt;/button&gt;</t>
-    </r>
   </si>
   <si>
     <t>`https://element.eleme.io/#/en-US/component/date-picker</t>
@@ -7774,17 +7640,261 @@
   <si>
     <t>Результат должен быть</t>
   </si>
+  <si>
+    <t>Вариант 3</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                &lt;el-button
+                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :style="condformattingobj.colorformatting?.active ? activeStyleColor : {}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                &gt;
+                &lt;/el-button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">data() {
+        return {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">            activeStyleColor: {
+                backgroundColor: "#409EFF",
+                borderColor: "#409EFF",
+                color: "#fff",
+            },
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">        };
+    },</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                &lt;el-button
+                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :style="{backgroundColor: "#409EFF",}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                &gt;
+                &lt;/el-button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                &lt;el-button
+                   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :style="{backgroundColor: item.length === 0 ? "#409EFF" : "#FFF",}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                &gt;
+                &lt;/el-button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                      &lt;button 
+                              v-bind:class="
+                              {
+                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'btn-danger': colorEdit &amp;&amp; baseSettings.editUserCurrentSetting,
+                                'btn-default': !colorEdit || !baseSettings.editUserCurrentSetting, 
+                                'btn-primary': colorEdit &amp;&amp; !baseSettings.editUserCurrentSetting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                              }
+                              "
+                      &lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                      &lt;button 
+                              v-bind:class="
+                              [
+                                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'custom_class_1',
+                                {'btn-danger': !colorEdit || !baseSettings.editUserCurrentSetting}, 
+                                'custom_class_2'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                              ]
+                              "
+                      &lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                      &lt;button 
+                              v-bind:class=" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "
+                      &lt;/button&gt;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8206,10 +8316,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -8220,20 +8330,20 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -8245,7 +8355,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -8254,89 +8364,83 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="18" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="26" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="34" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -8345,37 +8449,49 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -8384,40 +8500,25 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="40" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{141A142D-D8A7-43F9-B8D2-54AA311FA1CB}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9497,35 +9598,35 @@
       <selection activeCell="B283" sqref="B283"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="71.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="64.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="7.88671875" style="7" customWidth="1"/>
-    <col min="11" max="11" width="39.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="72.5546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="7.88671875" style="7" customWidth="1"/>
-    <col min="16" max="16" width="56.88671875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="46.6640625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="2" customWidth="1"/>
-    <col min="19" max="19" width="49.109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" style="8"/>
-    <col min="21" max="21" width="67.6640625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="68.44140625" style="1" customWidth="1"/>
-    <col min="23" max="24" width="59.44140625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="59.5546875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="41.33203125" style="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="50.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="71.08984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.36328125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="43.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="64.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="7.90625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="39.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="72.54296875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="7.90625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="56.90625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="46.6328125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="49.08984375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6328125" style="8"/>
+    <col min="21" max="21" width="67.6328125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="68.453125" style="1" customWidth="1"/>
+    <col min="23" max="24" width="59.453125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="59.54296875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="41.36328125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22">
@@ -9573,7 +9674,7 @@
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -9582,12 +9683,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="28.8">
+    <row r="7" spans="1:22" ht="29">
       <c r="C7" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="100.8">
+    <row r="8" spans="1:22" ht="101.5">
       <c r="B8" s="2" t="s">
         <v>216</v>
       </c>
@@ -9631,7 +9732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="28.8">
+    <row r="12" spans="1:22" ht="29">
       <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
@@ -9642,7 +9743,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="28.8">
+    <row r="13" spans="1:22" ht="29">
       <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
@@ -9650,7 +9751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="28.8">
+    <row r="14" spans="1:22" ht="29">
       <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
@@ -9658,7 +9759,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="28.8">
+    <row r="15" spans="1:22" ht="29">
       <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
@@ -9666,7 +9767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="28.8">
+    <row r="16" spans="1:22" ht="29">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -9680,7 +9781,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="100.8">
+    <row r="17" spans="1:22" ht="101.5">
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
@@ -9691,7 +9792,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="28.8">
+    <row r="18" spans="1:22" ht="29">
       <c r="A18" s="10" t="s">
         <v>29</v>
       </c>
@@ -9702,7 +9803,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="100.8">
+    <row r="19" spans="1:22" ht="101.5">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -9710,7 +9811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="100.8">
+    <row r="20" spans="1:22" ht="101.5">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -9748,7 +9849,7 @@
       <c r="U23" s="1"/>
       <c r="V23" s="2"/>
     </row>
-    <row r="24" spans="1:22" ht="28.8">
+    <row r="24" spans="1:22" ht="29">
       <c r="A24" s="10" t="s">
         <v>36</v>
       </c>
@@ -9764,7 +9865,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="57.6">
+    <row r="26" spans="1:22" ht="58">
       <c r="B26" s="2" t="s">
         <v>37</v>
       </c>
@@ -9772,7 +9873,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="28.8">
+    <row r="27" spans="1:22" ht="29">
       <c r="C27" s="9" t="s">
         <v>43</v>
       </c>
@@ -9785,7 +9886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="72">
+    <row r="29" spans="1:22" ht="72.5">
       <c r="B29" s="2" t="s">
         <v>35</v>
       </c>
@@ -9801,7 +9902,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="129.6">
+    <row r="31" spans="1:22" ht="130.5">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -9812,7 +9913,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="57.6">
+    <row r="32" spans="1:22" ht="58">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -9823,7 +9924,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="115.2">
+    <row r="33" spans="1:4" ht="116">
       <c r="B33" s="2" t="s">
         <v>50</v>
       </c>
@@ -9831,7 +9932,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="115.2">
+    <row r="34" spans="1:4" ht="116">
       <c r="A34" s="1" t="s">
         <v>53</v>
       </c>
@@ -9845,7 +9946,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="72">
+    <row r="35" spans="1:4" ht="72.5">
       <c r="A35" s="1" t="s">
         <v>57</v>
       </c>
@@ -9856,7 +9957,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="115.2">
+    <row r="36" spans="1:4" ht="116">
       <c r="C36" s="13" t="s">
         <v>63</v>
       </c>
@@ -9873,15 +9974,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="43.2">
-      <c r="B38" s="18" t="s">
+    <row r="38" spans="1:4" ht="43.5">
+      <c r="B38" s="17" t="s">
         <v>190</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="187.2">
+    <row r="39" spans="1:4" ht="188.5">
       <c r="B39" s="2" t="s">
         <v>120</v>
       </c>
@@ -9889,7 +9990,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8">
+    <row r="40" spans="1:4" ht="29">
       <c r="C40" s="13" t="s">
         <v>117</v>
       </c>
@@ -9907,7 +10008,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="28.8">
+    <row r="43" spans="1:4" ht="29">
       <c r="A43" s="2" t="s">
         <v>61</v>
       </c>
@@ -9915,12 +10016,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="28.8">
+    <row r="44" spans="1:4" ht="29">
       <c r="C44" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.8">
+    <row r="45" spans="1:4" ht="29">
       <c r="A45" s="2" t="s">
         <v>62</v>
       </c>
@@ -9938,7 +10039,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="86.4">
+    <row r="48" spans="1:4" ht="87">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -9957,8 +10058,8 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="216">
-      <c r="A50" s="18" t="s">
+    <row r="50" spans="1:22" ht="217.5">
+      <c r="A50" s="17" t="s">
         <v>183</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -9974,7 +10075,7 @@
       </c>
       <c r="C51" s="13"/>
     </row>
-    <row r="52" spans="1:22" ht="86.4">
+    <row r="52" spans="1:22" ht="87">
       <c r="A52" s="2" t="s">
         <v>179</v>
       </c>
@@ -9985,7 +10086,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="43.2">
+    <row r="53" spans="1:22" ht="43.5">
       <c r="C53" s="13" t="s">
         <v>67</v>
       </c>
@@ -10030,7 +10131,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="28.8">
+    <row r="62" spans="1:22" ht="29">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
@@ -10044,7 +10145,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="57.6">
+    <row r="63" spans="1:22" ht="58">
       <c r="A63" s="1" t="s">
         <v>81</v>
       </c>
@@ -10055,7 +10156,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:22" ht="28.8">
+    <row r="64" spans="1:22" ht="29">
       <c r="A64" s="13" t="s">
         <v>98</v>
       </c>
@@ -10067,7 +10168,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="28.8">
+    <row r="65" spans="1:22" ht="29">
       <c r="A65" s="1" t="s">
         <v>102</v>
       </c>
@@ -10084,7 +10185,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="72">
+    <row r="67" spans="1:22" ht="72.5">
       <c r="B67" s="2" t="s">
         <v>94</v>
       </c>
@@ -10092,12 +10193,12 @@
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="144">
+    <row r="68" spans="1:22" ht="145">
       <c r="C68" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="115.2">
+    <row r="69" spans="1:22" ht="116">
       <c r="C69" s="13" t="s">
         <v>95</v>
       </c>
@@ -10110,7 +10211,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="43.2">
+    <row r="71" spans="1:22" ht="43.5">
       <c r="A71" s="1" t="s">
         <v>90</v>
       </c>
@@ -10121,7 +10222,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="28.8">
+    <row r="72" spans="1:22" ht="29">
       <c r="A72" s="1" t="s">
         <v>104</v>
       </c>
@@ -10130,7 +10231,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="129.6">
+    <row r="73" spans="1:22" ht="130.5">
       <c r="A73" s="1" t="s">
         <v>105</v>
       </c>
@@ -10141,7 +10242,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="100.8">
+    <row r="74" spans="1:22" ht="101.5">
       <c r="A74" s="1" t="s">
         <v>105</v>
       </c>
@@ -10152,7 +10253,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="72">
+    <row r="75" spans="1:22" ht="72.5">
       <c r="B75" s="2" t="s">
         <v>109</v>
       </c>
@@ -10206,7 +10307,7 @@
       <c r="U79" s="1"/>
       <c r="V79" s="2"/>
     </row>
-    <row r="80" spans="1:22" ht="409.6">
+    <row r="80" spans="1:22" ht="409.5">
       <c r="C80" s="2" t="s">
         <v>146</v>
       </c>
@@ -10225,7 +10326,7 @@
       <c r="U81" s="1"/>
       <c r="V81" s="2"/>
     </row>
-    <row r="82" spans="1:22" ht="86.4">
+    <row r="82" spans="1:22" ht="87">
       <c r="A82" s="1" t="s">
         <v>123</v>
       </c>
@@ -10236,7 +10337,7 @@
       <c r="U82" s="1"/>
       <c r="V82" s="2"/>
     </row>
-    <row r="83" spans="1:22" ht="43.2">
+    <row r="83" spans="1:22" ht="43.5">
       <c r="A83" s="1" t="s">
         <v>124</v>
       </c>
@@ -10256,7 +10357,7 @@
       <c r="U84" s="1"/>
       <c r="V84" s="2"/>
     </row>
-    <row r="85" spans="1:22" ht="28.8">
+    <row r="85" spans="1:22" ht="29">
       <c r="A85" s="1" t="s">
         <v>125</v>
       </c>
@@ -10267,7 +10368,7 @@
       <c r="U85" s="1"/>
       <c r="V85" s="2"/>
     </row>
-    <row r="86" spans="1:22" ht="28.8">
+    <row r="86" spans="1:22" ht="29">
       <c r="A86" s="1" t="s">
         <v>126</v>
       </c>
@@ -10278,7 +10379,7 @@
       <c r="U86" s="1"/>
       <c r="V86" s="2"/>
     </row>
-    <row r="87" spans="1:22" ht="158.4">
+    <row r="87" spans="1:22" ht="159.5">
       <c r="B87" s="2" t="s">
         <v>156</v>
       </c>
@@ -10298,7 +10399,7 @@
       <c r="U88" s="1"/>
       <c r="V88" s="2"/>
     </row>
-    <row r="89" spans="1:22" ht="28.8">
+    <row r="89" spans="1:22" ht="29">
       <c r="A89" s="1" t="s">
         <v>137</v>
       </c>
@@ -10312,7 +10413,7 @@
       <c r="U89" s="1"/>
       <c r="V89" s="2"/>
     </row>
-    <row r="90" spans="1:22" ht="28.8">
+    <row r="90" spans="1:22" ht="29">
       <c r="A90" s="1" t="s">
         <v>139</v>
       </c>
@@ -10334,7 +10435,7 @@
       <c r="U91" s="1"/>
       <c r="V91" s="2"/>
     </row>
-    <row r="92" spans="1:22" ht="28.8">
+    <row r="92" spans="1:22" ht="29">
       <c r="A92" s="1" t="s">
         <v>144</v>
       </c>
@@ -10345,21 +10446,21 @@
       <c r="U92" s="1"/>
       <c r="V92" s="2"/>
     </row>
-    <row r="93" spans="1:22" ht="86.4">
+    <row r="93" spans="1:22" ht="87">
       <c r="B93" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D93" s="16" t="s">
+      <c r="D93" s="1" t="s">
         <v>159</v>
       </c>
       <c r="P93" s="1"/>
       <c r="U93" s="1"/>
       <c r="V93" s="2"/>
     </row>
-    <row r="94" spans="1:22" ht="28.8">
+    <row r="94" spans="1:22" ht="29">
       <c r="A94" s="1" t="s">
         <v>145</v>
       </c>
@@ -10370,15 +10471,15 @@
       <c r="U94" s="1"/>
       <c r="V94" s="2"/>
     </row>
-    <row r="95" spans="1:22" ht="28.8">
-      <c r="C95" s="17" t="s">
+    <row r="95" spans="1:22" ht="29">
+      <c r="C95" s="16" t="s">
         <v>162</v>
       </c>
       <c r="P95" s="1"/>
       <c r="U95" s="1"/>
       <c r="V95" s="2"/>
     </row>
-    <row r="96" spans="1:22" ht="374.4">
+    <row r="96" spans="1:22" ht="377">
       <c r="A96" s="2" t="s">
         <v>169</v>
       </c>
@@ -10392,7 +10493,7 @@
       <c r="U96" s="1"/>
       <c r="V96" s="2"/>
     </row>
-    <row r="97" spans="1:22" ht="409.6">
+    <row r="97" spans="1:22" ht="409.5">
       <c r="B97" s="2" t="s">
         <v>164</v>
       </c>
@@ -10403,7 +10504,7 @@
       <c r="U97" s="1"/>
       <c r="V97" s="2"/>
     </row>
-    <row r="98" spans="1:22" ht="409.6">
+    <row r="98" spans="1:22" ht="409.5">
       <c r="B98" s="2" t="s">
         <v>166</v>
       </c>
@@ -10425,7 +10526,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="101" spans="1:22" ht="28.8">
+    <row r="101" spans="1:22" ht="29">
       <c r="A101" s="1" t="s">
         <v>148</v>
       </c>
@@ -10468,7 +10569,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="105" spans="1:22" ht="43.2">
+    <row r="105" spans="1:22" ht="43.5">
       <c r="A105" s="1" t="s">
         <v>151</v>
       </c>
@@ -10479,27 +10580,27 @@
         <v>153</v>
       </c>
     </row>
-    <row r="106" spans="1:22" ht="28.8">
+    <row r="106" spans="1:22" ht="29">
       <c r="A106" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="C106" s="18" t="s">
+      <c r="C106" s="17" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="107" spans="1:22" ht="57.6">
+    <row r="107" spans="1:22" ht="58">
       <c r="A107" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C107" s="18" t="s">
+      <c r="C107" s="17" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="108" spans="1:22" ht="115.2">
+    <row r="108" spans="1:22" ht="116">
       <c r="B108" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C108" s="18" t="s">
+      <c r="C108" s="17" t="s">
         <v>232</v>
       </c>
       <c r="D108" s="2" t="s">
@@ -10514,61 +10615,61 @@
         <v>171</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="57.6">
-      <c r="A113" s="18" t="s">
+    <row r="113" spans="1:4" ht="58">
+      <c r="A113" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="17" t="s">
         <v>198</v>
       </c>
-      <c r="C113" s="18" t="s">
+      <c r="C113" s="17" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="72">
-      <c r="A114" s="18"/>
-      <c r="B114" s="18"/>
-      <c r="C114" s="18" t="s">
+    <row r="114" spans="1:4" ht="72.5">
+      <c r="A114" s="17"/>
+      <c r="B114" s="17"/>
+      <c r="C114" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="28.8">
+    <row r="115" spans="1:4" ht="29">
       <c r="B115" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C115" s="18" t="s">
+      <c r="C115" s="17" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="43.2">
+    <row r="116" spans="1:4" ht="43.5">
       <c r="B116" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C116" s="18" t="s">
+      <c r="C116" s="17" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="259.2">
+    <row r="117" spans="1:4" ht="261">
       <c r="B117" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="C117" s="18" t="s">
+      <c r="C117" s="17" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="28.8">
+    <row r="118" spans="1:4" ht="29">
       <c r="B118" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C118" s="18" t="s">
+      <c r="C118" s="17" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="216">
+    <row r="119" spans="1:4" ht="217.5">
       <c r="B119" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C119" s="18" t="s">
+      <c r="C119" s="17" t="s">
         <v>220</v>
       </c>
     </row>
@@ -10577,32 +10678,32 @@
         <v>182</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="409.6">
+    <row r="121" spans="1:4" ht="409.5">
       <c r="B121" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C121" s="18" t="s">
+      <c r="C121" s="17" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="72">
-      <c r="A122" s="33" t="s">
+    <row r="122" spans="1:4" ht="72.5">
+      <c r="A122" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="C122" s="18" t="s">
+      <c r="C122" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="374.4">
-      <c r="C123" s="18" t="s">
+    <row r="123" spans="1:4" ht="377">
+      <c r="C123" s="17" t="s">
         <v>224</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="331.2">
-      <c r="C124" s="18" t="s">
+    <row r="124" spans="1:4" ht="333.5">
+      <c r="C124" s="17" t="s">
         <v>227</v>
       </c>
       <c r="D124" s="2" t="s">
@@ -10617,14 +10718,14 @@
         <v>193</v>
       </c>
     </row>
-    <row r="126" spans="1:4" ht="115.2">
-      <c r="A126" s="18" t="s">
+    <row r="126" spans="1:4" ht="116">
+      <c r="A126" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B126" s="18" t="s">
+      <c r="B126" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="C126" s="18" t="s">
+      <c r="C126" s="17" t="s">
         <v>211</v>
       </c>
     </row>
@@ -10636,18 +10737,18 @@
         <v>199</v>
       </c>
     </row>
-    <row r="128" spans="1:4" ht="158.4">
+    <row r="128" spans="1:4" ht="159.5">
       <c r="B128" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="C128" s="18" t="s">
+      <c r="C128" s="17" t="s">
         <v>213</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="129" spans="1:22" ht="144">
+    <row r="129" spans="1:22" ht="145">
       <c r="D129" s="2" t="s">
         <v>215</v>
       </c>
@@ -10687,25 +10788,25 @@
         <v>289</v>
       </c>
     </row>
-    <row r="135" spans="1:22" ht="57.6">
+    <row r="135" spans="1:22" ht="58">
       <c r="A135" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B135" s="17" t="s">
+      <c r="B135" s="16" t="s">
         <v>290</v>
       </c>
-      <c r="C135" s="18" t="s">
+      <c r="C135" s="17" t="s">
         <v>196</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="136" spans="1:22" ht="144">
+    <row r="136" spans="1:22" ht="145">
       <c r="A136" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B136" s="18" t="s">
+      <c r="B136" s="17" t="s">
         <v>291</v>
       </c>
       <c r="C136" s="2" t="s">
@@ -10716,19 +10817,19 @@
       </c>
     </row>
     <row r="137" spans="1:22">
-      <c r="C137" s="18"/>
+      <c r="C137" s="17"/>
     </row>
     <row r="138" spans="1:22">
-      <c r="C138" s="18"/>
+      <c r="C138" s="17"/>
     </row>
     <row r="139" spans="1:22">
-      <c r="C139" s="18"/>
+      <c r="C139" s="17"/>
     </row>
     <row r="140" spans="1:22">
-      <c r="C140" s="18"/>
+      <c r="C140" s="17"/>
     </row>
     <row r="141" spans="1:22">
-      <c r="C141" s="18"/>
+      <c r="C141" s="17"/>
     </row>
     <row r="142" spans="1:22">
       <c r="A142" s="3"/>
@@ -10768,11 +10869,11 @@
         <v>235</v>
       </c>
     </row>
-    <row r="145" spans="1:4" ht="158.4">
+    <row r="145" spans="1:4" ht="145">
       <c r="B145" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C145" s="18" t="s">
+      <c r="C145" s="17" t="s">
         <v>237</v>
       </c>
     </row>
@@ -10788,11 +10889,11 @@
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
     </row>
-    <row r="148" spans="1:4" ht="72">
+    <row r="148" spans="1:4" ht="72.5">
       <c r="B148" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C148" s="18" t="s">
+      <c r="C148" s="17" t="s">
         <v>248</v>
       </c>
     </row>
@@ -10803,34 +10904,34 @@
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
     </row>
-    <row r="150" spans="1:4" ht="187.2">
-      <c r="A150" s="36"/>
+    <row r="150" spans="1:4" ht="188.5">
+      <c r="A150" s="33"/>
       <c r="B150" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C150" s="36" t="s">
+      <c r="C150" s="33" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="57.6">
+    <row r="151" spans="1:4" ht="58">
       <c r="A151" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="C151" s="18" t="s">
+      <c r="C151" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="D151" s="18" t="s">
+      <c r="D151" s="17" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="216">
+    <row r="152" spans="1:4" ht="217.5">
       <c r="A152" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="C152" s="36" t="s">
+      <c r="C152" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="D152" s="18" t="s">
+      <c r="D152" s="17" t="s">
         <v>283</v>
       </c>
     </row>
@@ -10841,48 +10942,47 @@
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
     </row>
-    <row r="154" spans="1:4" ht="144">
-      <c r="A154" s="16"/>
+    <row r="154" spans="1:4" ht="145">
       <c r="B154" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C154" s="18" t="s">
+      <c r="C154" s="17" t="s">
         <v>270</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="230.4">
+    <row r="155" spans="1:4" ht="232">
       <c r="A155" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="C155" s="18" t="s">
+      <c r="C155" s="17" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="144">
+    <row r="156" spans="1:4" ht="145">
       <c r="A156" s="1" t="s">
         <v>272</v>
       </c>
       <c r="B156" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="C156" s="18" t="s">
+      <c r="C156" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="D156" s="18" t="s">
+      <c r="D156" s="17" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="43.2">
+    <row r="157" spans="1:4" ht="43.5">
       <c r="B157" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="C157" s="18" t="s">
+      <c r="C157" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="D157" s="18"/>
+      <c r="D157" s="17"/>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="11" t="s">
@@ -10894,36 +10994,36 @@
         <v>292</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="244.8">
+    <row r="159" spans="1:4" ht="246.5">
       <c r="B159" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C159" s="18" t="s">
+      <c r="C159" s="17" t="s">
         <v>252</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="331.2">
+    <row r="160" spans="1:4" ht="333.5">
       <c r="A160" s="1" t="s">
         <v>295</v>
       </c>
       <c r="B160" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C160" s="18" t="s">
+      <c r="C160" s="17" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="161" spans="1:22" ht="115.2">
+    <row r="161" spans="1:22" ht="116">
       <c r="A161" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C161" s="18" t="s">
+      <c r="C161" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="D161" s="18" t="s">
+      <c r="D161" s="17" t="s">
         <v>297</v>
       </c>
     </row>
@@ -10934,21 +11034,21 @@
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
     </row>
-    <row r="163" spans="1:22" ht="172.8">
+    <row r="163" spans="1:22" ht="174">
       <c r="B163" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="C163" s="18" t="s">
+      <c r="C163" s="17" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="164" spans="1:22">
-      <c r="A164" s="34" t="s">
+      <c r="A164" s="31" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="165" spans="1:22" ht="43.2">
-      <c r="C165" s="18" t="s">
+    <row r="165" spans="1:22" ht="43.5">
+      <c r="C165" s="17" t="s">
         <v>254</v>
       </c>
     </row>
@@ -10956,49 +11056,49 @@
       <c r="A166" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C166" s="35" t="s">
+      <c r="C166" s="32" t="s">
         <v>266</v>
       </c>
       <c r="D166" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="167" spans="1:22" ht="144">
+    <row r="167" spans="1:22" ht="145">
       <c r="A167" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B167" s="18" t="s">
+      <c r="B167" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="C167" s="18" t="s">
+      <c r="C167" s="17" t="s">
         <v>260</v>
       </c>
       <c r="D167" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="168" spans="1:22" ht="409.6">
+    <row r="168" spans="1:22" ht="409.5">
       <c r="A168" s="2" t="s">
         <v>256</v>
       </c>
       <c r="B168" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="C168" s="18" t="s">
+      <c r="C168" s="17" t="s">
         <v>257</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="169" spans="1:22" ht="409.6">
-      <c r="A169" s="18" t="s">
+    <row r="169" spans="1:22" ht="409.5">
+      <c r="A169" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B169" s="18" t="s">
+      <c r="B169" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="C169" s="18" t="s">
+      <c r="C169" s="17" t="s">
         <v>264</v>
       </c>
     </row>
@@ -11078,39 +11178,39 @@
         <v>306</v>
       </c>
     </row>
-    <row r="183" spans="1:22" ht="100.8">
+    <row r="183" spans="1:22" ht="101.5">
       <c r="A183" s="1" t="s">
         <v>309</v>
       </c>
       <c r="B183" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C183" s="37" t="s">
+      <c r="C183" s="34" t="s">
         <v>310</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="184" spans="1:22" ht="100.8">
+    <row r="184" spans="1:22" ht="101.5">
       <c r="A184" s="1" t="s">
         <v>312</v>
       </c>
       <c r="B184" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C184" s="37" t="s">
+      <c r="C184" s="34" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="185" spans="1:22" ht="129.6">
+    <row r="185" spans="1:22" ht="130.5">
       <c r="A185" s="1" t="s">
         <v>315</v>
       </c>
       <c r="B185" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C185" s="53" t="s">
+      <c r="C185" s="50" t="s">
         <v>316</v>
       </c>
       <c r="D185" s="1" t="s">
@@ -11152,25 +11252,25 @@
         <v>324</v>
       </c>
     </row>
-    <row r="191" spans="1:22" ht="72">
+    <row r="191" spans="1:22" ht="72.5">
       <c r="A191" s="1" t="s">
         <v>319</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="C191" s="37" t="s">
+      <c r="C191" s="34" t="s">
         <v>320</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="192" spans="1:22" ht="259.2">
+    <row r="192" spans="1:22" ht="261">
       <c r="B192" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C192" s="37" t="s">
+      <c r="C192" s="34" t="s">
         <v>323</v>
       </c>
       <c r="D192" s="1" t="s">
@@ -11216,10 +11316,10 @@
       </c>
     </row>
     <row r="197" spans="1:22">
-      <c r="A197" s="38" t="s">
+      <c r="A197" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="C197" s="39" t="s">
+      <c r="C197" s="36" t="s">
         <v>332</v>
       </c>
       <c r="D197" s="1" t="s">
@@ -11230,7 +11330,7 @@
       <c r="A198" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C198" s="39" t="s">
+      <c r="C198" s="36" t="s">
         <v>334</v>
       </c>
     </row>
@@ -11238,7 +11338,7 @@
       <c r="A199" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C199" s="39" t="s">
+      <c r="C199" s="36" t="s">
         <v>335</v>
       </c>
     </row>
@@ -11250,8 +11350,8 @@
         <v>336</v>
       </c>
     </row>
-    <row r="201" spans="1:22" ht="409.6">
-      <c r="C201" s="53" t="s">
+    <row r="201" spans="1:22" ht="409.5">
+      <c r="C201" s="50" t="s">
         <v>358</v>
       </c>
     </row>
@@ -11260,11 +11360,11 @@
         <v>339</v>
       </c>
     </row>
-    <row r="203" spans="1:22" ht="115.2">
+    <row r="203" spans="1:22" ht="116">
       <c r="B203" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C203" s="39" t="s">
+      <c r="C203" s="36" t="s">
         <v>337</v>
       </c>
     </row>
@@ -11273,8 +11373,8 @@
         <v>342</v>
       </c>
     </row>
-    <row r="205" spans="1:22" ht="72">
-      <c r="C205" s="40" t="s">
+    <row r="205" spans="1:22" ht="72.5">
+      <c r="C205" s="37" t="s">
         <v>343</v>
       </c>
       <c r="D205" s="1" t="s">
@@ -11285,27 +11385,25 @@
       <c r="A206" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="C206" s="40" t="s">
+      <c r="C206" s="37" t="s">
         <v>346</v>
       </c>
-      <c r="D206" s="16"/>
-    </row>
-    <row r="207" spans="1:22" ht="144">
-      <c r="C207" s="42" t="s">
+    </row>
+    <row r="207" spans="1:22" ht="145">
+      <c r="C207" s="39" t="s">
         <v>353</v>
       </c>
-      <c r="D207" s="16"/>
     </row>
     <row r="208" spans="1:22">
       <c r="A208" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="C208" s="40" t="s">
+      <c r="C208" s="37" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="28.8">
-      <c r="C209" s="42" t="s">
+    <row r="209" spans="1:4" ht="29">
+      <c r="C209" s="39" t="s">
         <v>347</v>
       </c>
     </row>
@@ -11313,32 +11411,32 @@
       <c r="A210" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="C210" s="40" t="s">
+      <c r="C210" s="37" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="72">
-      <c r="C211" s="40" t="s">
+    <row r="211" spans="1:4" ht="72.5">
+      <c r="C211" s="37" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="212" spans="1:4">
-      <c r="A212" s="41" t="s">
+      <c r="A212" s="38" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="213" spans="1:4">
-      <c r="C213" s="40" t="s">
+      <c r="C213" s="37" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="214" spans="1:4">
-      <c r="C214" s="40" t="s">
+      <c r="C214" s="37" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="215" spans="1:4">
-      <c r="C215" s="40" t="s">
+      <c r="C215" s="37" t="s">
         <v>351</v>
       </c>
     </row>
@@ -11347,8 +11445,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="158.4">
-      <c r="B217" s="40" t="s">
+    <row r="217" spans="1:4" ht="159.5">
+      <c r="B217" s="37" t="s">
         <v>354</v>
       </c>
     </row>
@@ -11357,22 +11455,22 @@
         <v>338</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="144">
+    <row r="219" spans="1:4" ht="145">
       <c r="B219" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="C219" s="40" t="s">
+      <c r="C219" s="37" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="86.4">
+    <row r="220" spans="1:4" ht="87">
       <c r="B220" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C220" s="42" t="s">
+      <c r="C220" s="39" t="s">
         <v>360</v>
       </c>
-      <c r="D220" s="16" t="s">
+      <c r="D220" s="1" t="s">
         <v>357</v>
       </c>
     </row>
@@ -11380,26 +11478,26 @@
       <c r="A221" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="D221" s="16" t="s">
+      <c r="D221" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="72">
+    <row r="222" spans="1:4" ht="72.5">
       <c r="A222" s="1" t="s">
         <v>373</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="C222" s="42" t="s">
+      <c r="C222" s="39" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="158.4">
+    <row r="223" spans="1:4" ht="159.5">
       <c r="B223" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C223" s="42" t="s">
+      <c r="C223" s="39" t="s">
         <v>365</v>
       </c>
     </row>
@@ -11407,15 +11505,15 @@
       <c r="A224" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="D224" s="16" t="s">
+      <c r="D224" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="225" spans="1:22" ht="187.2">
+    <row r="225" spans="1:22" ht="188.5">
       <c r="B225" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="C225" s="42" t="s">
+      <c r="C225" s="39" t="s">
         <v>367</v>
       </c>
     </row>
@@ -11424,61 +11522,61 @@
         <v>369</v>
       </c>
     </row>
-    <row r="227" spans="1:22" ht="216">
+    <row r="227" spans="1:22" ht="217.5">
       <c r="A227" s="2" t="s">
         <v>374</v>
       </c>
       <c r="B227" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C227" s="42" t="s">
+      <c r="C227" s="39" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="228" spans="1:22" ht="201.6">
+    <row r="228" spans="1:22" ht="203">
       <c r="A228" s="1" t="s">
         <v>379</v>
       </c>
       <c r="B228" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="C228" s="42" t="s">
+      <c r="C228" s="39" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="229" spans="1:22" ht="158.4">
-      <c r="A229" s="43" t="s">
+    <row r="229" spans="1:22" ht="159.5">
+      <c r="A229" s="40" t="s">
         <v>383</v>
       </c>
-      <c r="C229" s="43" t="s">
+      <c r="C229" s="40" t="s">
         <v>384</v>
       </c>
-      <c r="D229" s="16" t="s">
+      <c r="D229" s="1" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="230" spans="1:22" ht="28.8">
-      <c r="A230" s="44" t="s">
+    <row r="230" spans="1:22" ht="29">
+      <c r="A230" s="41" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="231" spans="1:22" ht="144">
+    <row r="231" spans="1:22" ht="145">
       <c r="B231" s="1"/>
       <c r="C231" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="D231" s="43" t="s">
+      <c r="D231" s="40" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="232" spans="1:22">
-      <c r="A232" s="41" t="s">
+      <c r="A232" s="38" t="s">
         <v>349</v>
       </c>
       <c r="C232" s="1"/>
-      <c r="D232" s="43"/>
-    </row>
-    <row r="233" spans="1:22" ht="72">
+      <c r="D232" s="40"/>
+    </row>
+    <row r="233" spans="1:22" ht="72.5">
       <c r="C233" s="2" t="s">
         <v>385</v>
       </c>
@@ -11543,7 +11641,7 @@
       <c r="S243" s="5"/>
       <c r="U243" s="5"/>
     </row>
-    <row r="244" spans="1:22" ht="28.8">
+    <row r="244" spans="1:22" ht="29">
       <c r="A244" s="1" t="s">
         <v>390</v>
       </c>
@@ -11562,78 +11660,78 @@
         <v>392</v>
       </c>
     </row>
-    <row r="246" spans="1:22" ht="57.6">
-      <c r="C246" s="45" t="s">
+    <row r="246" spans="1:22" ht="58">
+      <c r="C246" s="42" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="247" spans="1:22" ht="28.8">
-      <c r="A247" s="44" t="s">
+    <row r="247" spans="1:22" ht="29">
+      <c r="A247" s="41" t="s">
         <v>407</v>
       </c>
-      <c r="C247" s="45"/>
-    </row>
-    <row r="248" spans="1:22" ht="288">
+      <c r="C247" s="42"/>
+    </row>
+    <row r="248" spans="1:22" ht="290">
       <c r="A248" s="1" t="s">
         <v>400</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="C248" s="46" t="s">
+      <c r="C248" s="43" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="249" spans="1:22" ht="302.39999999999998">
+    <row r="249" spans="1:22" ht="304.5">
       <c r="A249" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="C249" s="45" t="s">
+      <c r="C249" s="42" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="250" spans="1:22" ht="409.6">
+    <row r="250" spans="1:22" ht="409.5">
       <c r="A250" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="C250" s="45" t="s">
+      <c r="C250" s="42" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="251" spans="1:22" ht="273.60000000000002">
+    <row r="251" spans="1:22" ht="275.5">
       <c r="A251" s="1" t="s">
         <v>406</v>
       </c>
       <c r="B251" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="C251" s="45" t="s">
+      <c r="C251" s="42" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="252" spans="1:22">
-      <c r="A252" s="41" t="s">
+      <c r="A252" s="38" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="253" spans="1:22" ht="86.4">
+    <row r="253" spans="1:22" ht="87">
       <c r="B253" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="C253" s="45" t="s">
+      <c r="C253" s="42" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="254" spans="1:22" ht="28.8">
-      <c r="A254" s="44" t="s">
+    <row r="254" spans="1:22" ht="29">
+      <c r="A254" s="41" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="255" spans="1:22" ht="316.8">
+    <row r="255" spans="1:22" ht="319">
       <c r="A255" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="C255" s="45" t="s">
+      <c r="C255" s="42" t="s">
         <v>409</v>
       </c>
     </row>
@@ -11645,25 +11743,25 @@
         <v>412</v>
       </c>
     </row>
-    <row r="257" spans="1:22" ht="409.6">
+    <row r="257" spans="1:22" ht="409.5">
       <c r="A257" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="B257" s="45" t="s">
+      <c r="B257" s="42" t="s">
         <v>416</v>
       </c>
-      <c r="C257" s="45" t="s">
+      <c r="C257" s="42" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="258" spans="1:22" ht="288">
+    <row r="258" spans="1:22" ht="290">
       <c r="A258" s="1" t="s">
         <v>406</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="C258" s="45" t="s">
+      <c r="C258" s="42" t="s">
         <v>403</v>
       </c>
     </row>
@@ -11697,33 +11795,33 @@
       <c r="U261" s="1"/>
       <c r="V261" s="2"/>
     </row>
-    <row r="262" spans="1:22" ht="28.8">
-      <c r="C262" s="46" t="s">
+    <row r="262" spans="1:22" ht="29">
+      <c r="C262" s="43" t="s">
         <v>420</v>
       </c>
       <c r="D262" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="263" spans="1:22" ht="409.6">
+    <row r="263" spans="1:22" ht="409.5">
       <c r="A263" s="1" t="s">
         <v>338</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C263" s="46" t="s">
+      <c r="C263" s="43" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="264" spans="1:22" ht="360">
+    <row r="264" spans="1:22" ht="362.5">
       <c r="A264" s="1" t="s">
         <v>422</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="C264" s="46" t="s">
+      <c r="C264" s="43" t="s">
         <v>423</v>
       </c>
     </row>
@@ -11746,12 +11844,12 @@
       <c r="S266" s="5"/>
       <c r="U266" s="5"/>
     </row>
-    <row r="267" spans="1:22" ht="28.8">
+    <row r="267" spans="1:22" ht="29">
       <c r="A267" s="1" t="s">
         <v>425</v>
       </c>
       <c r="C267" s="12" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D267" s="1" t="s">
         <v>426</v>
@@ -11765,56 +11863,56 @@
         <v>438</v>
       </c>
     </row>
-    <row r="269" spans="1:22" ht="28.8">
+    <row r="269" spans="1:22" ht="29">
       <c r="A269" s="2" t="s">
         <v>429</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C269" s="47" t="s">
+      <c r="C269" s="44" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="270" spans="1:22" ht="28.8">
+    <row r="270" spans="1:22" ht="29">
       <c r="A270" s="2" t="s">
         <v>431</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="C270" s="47" t="s">
+      <c r="C270" s="44" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="271" spans="1:22" ht="28.8">
+    <row r="271" spans="1:22" ht="43.5">
       <c r="A271" s="2" t="s">
         <v>434</v>
       </c>
       <c r="B271" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="C271" s="47" t="s">
+      <c r="C271" s="44" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="272" spans="1:22">
-      <c r="A272" s="33" t="s">
+      <c r="A272" s="30" t="s">
         <v>437</v>
       </c>
       <c r="C272" s="1"/>
     </row>
-    <row r="273" spans="1:3" ht="28.8">
+    <row r="273" spans="1:3" ht="29">
       <c r="A273" s="2"/>
-      <c r="C273" s="47" t="s">
+      <c r="C273" s="44" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="274" spans="1:3" ht="57.6">
-      <c r="A274" s="47" t="s">
+    <row r="274" spans="1:3" ht="58">
+      <c r="A274" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="C274" s="47" t="s">
+      <c r="C274" s="44" t="s">
         <v>440</v>
       </c>
     </row>
@@ -11825,67 +11923,67 @@
       <c r="B275" s="2" t="s">
         <v>451</v>
       </c>
-      <c r="C275" s="47"/>
-    </row>
-    <row r="276" spans="1:3" ht="30">
+      <c r="C275" s="44"/>
+    </row>
+    <row r="276" spans="1:3" ht="32">
       <c r="A276" s="2" t="s">
         <v>447</v>
       </c>
       <c r="B276" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C276" s="48" t="s">
+      <c r="C276" s="45" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="277" spans="1:3" ht="60">
+    <row r="277" spans="1:3" ht="64">
       <c r="A277" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="C277" s="48" t="s">
+      <c r="C277" s="45" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="278" spans="1:3" ht="45">
+    <row r="278" spans="1:3" ht="48">
       <c r="A278" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="C278" s="48" t="s">
+      <c r="C278" s="45" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="279" spans="1:3" ht="28.8">
+    <row r="279" spans="1:3" ht="29">
       <c r="A279" s="2" t="s">
         <v>453</v>
       </c>
       <c r="B279" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="C279" s="47"/>
+      <c r="C279" s="44"/>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="2"/>
-      <c r="C280" s="47"/>
+      <c r="C280" s="44"/>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="2"/>
-      <c r="C281" s="47"/>
-    </row>
-    <row r="282" spans="1:3" ht="302.39999999999998">
+      <c r="C281" s="44"/>
+    </row>
+    <row r="282" spans="1:3" ht="304.5">
       <c r="B282" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="C282" s="49" t="s">
+      <c r="C282" s="46" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="283" spans="1:3" ht="216">
-      <c r="C283" s="49" t="s">
+    <row r="283" spans="1:3" ht="217.5">
+      <c r="C283" s="46" t="s">
         <v>441</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -11895,128 +11993,190 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF32088-FDD0-46A0-946F-1A7398394841}">
   <sheetPr>
-    <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="85.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="55" t="s">
-        <v>465</v>
-      </c>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
-    </row>
-    <row r="4" spans="1:22" s="19" customFormat="1">
-      <c r="A4" s="56" t="s">
-        <v>465</v>
-      </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="20"/>
-    </row>
-    <row r="5" spans="1:22" ht="374.4">
+      <c r="C3" s="51" t="s">
+        <v>463</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
+    </row>
+    <row r="4" spans="1:22" s="18" customFormat="1">
+      <c r="A4" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="19"/>
+    </row>
+    <row r="5" spans="1:22" ht="130.5">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="49" t="s">
-        <v>454</v>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>493</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="158.4">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="58">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="54" t="s">
-        <v>466</v>
-      </c>
-      <c r="D6" s="1"/>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>495</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="58">
+      <c r="A7" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>496</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="52" t="s">
+        <v>492</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" ht="58">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>499</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:22" ht="130.5">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>497</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:22" ht="145">
+      <c r="A11" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="C12" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -12029,148 +12189,148 @@
   </sheetPr>
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="61" t="s">
-        <v>485</v>
-      </c>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
-    </row>
-    <row r="4" spans="1:22" s="19" customFormat="1">
-      <c r="A4" s="62" t="s">
+      <c r="C3" s="57" t="s">
+        <v>482</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
+    </row>
+    <row r="4" spans="1:22" s="18" customFormat="1">
+      <c r="A4" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="30"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="20"/>
-    </row>
-    <row r="5" spans="1:22" s="19" customFormat="1">
-      <c r="A5" s="68" t="s">
-        <v>493</v>
-      </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="69" t="s">
-        <v>492</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="19"/>
+    </row>
+    <row r="5" spans="1:22" s="18" customFormat="1">
+      <c r="A5" s="62" t="s">
+        <v>490</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="63" t="s">
+        <v>489</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="19"/>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="59" t="s">
+        <v>486</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" ht="232">
+      <c r="A7" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="59" t="s">
+        <v>483</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:22" ht="409.5">
+      <c r="A8" s="60" t="s">
+        <v>487</v>
+      </c>
+      <c r="C8" s="61" t="s">
         <v>488</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="63" t="s">
-        <v>489</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:22" ht="230.4">
-      <c r="A7" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="63" t="s">
-        <v>486</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:22" ht="409.6">
-      <c r="A8" s="64" t="s">
-        <v>490</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>491</v>
       </c>
     </row>
   </sheetData>
@@ -12197,72 +12357,72 @@
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="57" t="s">
-        <v>468</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>467</v>
-      </c>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
+      <c r="C3" s="53" t="s">
+        <v>465</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>464</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12285,132 +12445,132 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="57" t="s">
-        <v>484</v>
-      </c>
-      <c r="D3" s="58"/>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
+      <c r="C3" s="53" t="s">
+        <v>481</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="60" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="129.6">
-      <c r="C5" s="59" t="s">
+      <c r="A4" s="56" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="130.5">
+      <c r="C5" s="55" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="217.5">
+      <c r="A6" s="54" t="s">
+        <v>470</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="319">
+      <c r="A7" s="54" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="216">
-      <c r="A6" s="58" t="s">
+      <c r="C7" s="55" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="362.5">
+      <c r="A8" s="54" t="s">
+        <v>474</v>
+      </c>
+      <c r="C8" s="55" t="s">
         <v>473</v>
       </c>
-      <c r="C6" s="59" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="316.8">
-      <c r="A7" s="58" t="s">
-        <v>474</v>
-      </c>
-      <c r="C7" s="59" t="s">
+    </row>
+    <row r="9" spans="1:22" ht="333.5">
+      <c r="A9" s="54" t="s">
+        <v>476</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="377">
+      <c r="A10" s="54" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" ht="360">
-      <c r="A8" s="58" t="s">
+      <c r="C10" s="55" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="56" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="409.5">
+      <c r="B12" s="55" t="s">
+        <v>478</v>
+      </c>
+      <c r="C12" s="55" t="s">
         <v>477</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="331.2">
-      <c r="A9" s="58" t="s">
-        <v>479</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" ht="374.4">
-      <c r="A10" s="58" t="s">
-        <v>478</v>
-      </c>
-      <c r="C10" s="59" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="60" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="409.6">
-      <c r="B12" s="59" t="s">
-        <v>481</v>
-      </c>
-      <c r="C12" s="59" t="s">
-        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -12433,136 +12593,136 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
-    </row>
-    <row r="4" spans="1:22" s="19" customFormat="1">
-      <c r="A4" s="28" t="s">
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
+    </row>
+    <row r="4" spans="1:22" s="18" customFormat="1">
+      <c r="A4" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="30"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="20"/>
-    </row>
-    <row r="5" spans="1:22" ht="86.4">
-      <c r="C5" s="21" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="19"/>
+    </row>
+    <row r="5" spans="1:22" ht="87">
+      <c r="C5" s="20" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="244.8">
-      <c r="C7" s="21" t="s">
+    <row r="7" spans="1:22" ht="246.5">
+      <c r="C7" s="20" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="43.2">
-      <c r="B9" s="21" t="s">
+    <row r="9" spans="1:22" ht="43.5">
+      <c r="B9" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="172.8">
-      <c r="B10" s="21" t="s">
+    <row r="10" spans="1:22" ht="174">
+      <c r="B10" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="29" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="244.8">
-      <c r="C12" s="21" t="s">
+    <row r="12" spans="1:22" ht="246.5">
+      <c r="C12" s="20" t="s">
         <v>210</v>
       </c>
     </row>
@@ -12586,105 +12746,105 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="24" t="s">
         <v>186</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
-    </row>
-    <row r="4" spans="1:22" s="19" customFormat="1">
-      <c r="A4" s="26" t="s">
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
+    </row>
+    <row r="4" spans="1:22" s="18" customFormat="1">
+      <c r="A4" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="21"/>
-      <c r="V4" s="20"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="25"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="19"/>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>189</v>
       </c>
     </row>
@@ -12708,98 +12868,98 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="36" style="20" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="21" customWidth="1"/>
-    <col min="3" max="3" width="71.21875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="20" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="20" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="19" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="20" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="20" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="19" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="21" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="21" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="21" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="22"/>
-    <col min="21" max="21" width="67.77734375" style="21" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="20" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="20" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="20" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="20" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="20" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="20"/>
+    <col min="1" max="1" width="36" style="19" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="71.1796875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="56.453125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.1796875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.08984375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="67.90625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="64.36328125" style="19" customWidth="1"/>
+    <col min="10" max="10" width="7.81640625" style="18" customWidth="1"/>
+    <col min="11" max="11" width="39.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.90625" style="19" customWidth="1"/>
+    <col min="13" max="13" width="72.6328125" style="19" customWidth="1"/>
+    <col min="14" max="14" width="43.90625" style="19" customWidth="1"/>
+    <col min="15" max="15" width="7.81640625" style="18" customWidth="1"/>
+    <col min="16" max="16" width="56.81640625" style="20" customWidth="1"/>
+    <col min="17" max="17" width="46.81640625" style="20" customWidth="1"/>
+    <col min="18" max="18" width="62.90625" style="20" customWidth="1"/>
+    <col min="19" max="19" width="49.1796875" style="19" customWidth="1"/>
+    <col min="20" max="20" width="8.81640625" style="21"/>
+    <col min="21" max="21" width="67.81640625" style="20" customWidth="1"/>
+    <col min="22" max="22" width="68.36328125" style="19" customWidth="1"/>
+    <col min="23" max="24" width="59.36328125" style="19" customWidth="1"/>
+    <col min="25" max="25" width="59.6328125" style="19" customWidth="1"/>
+    <col min="26" max="26" width="99.453125" style="19" customWidth="1"/>
+    <col min="27" max="27" width="41.1796875" style="19" customWidth="1"/>
+    <col min="28" max="16384" width="8.81640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66"/>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="47" t="s">
+        <v>455</v>
+      </c>
+      <c r="P3" s="19"/>
+      <c r="U3" s="19"/>
+      <c r="V3" s="20"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="49" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="409.5">
+      <c r="C5" s="48" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="333.5">
+      <c r="C6" s="48" t="s">
         <v>457</v>
       </c>
-      <c r="P3" s="20"/>
-      <c r="U3" s="20"/>
-      <c r="V3" s="21"/>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="52" t="s">
+    </row>
+    <row r="7" spans="1:22" ht="275.5">
+      <c r="C7" s="48" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="49" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="409.5">
+      <c r="C9" s="48" t="s">
         <v>461</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="409.6">
-      <c r="C5" s="51" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" ht="331.2">
-      <c r="C6" s="51" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" ht="273.60000000000002">
-      <c r="C7" s="51" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="52" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" ht="409.6">
-      <c r="C9" s="51" t="s">
-        <v>463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save 16 01 2026
</commit_message>
<xml_diff>
--- a/4 четверть_9_JavaScript_Vue.xlsx
+++ b/4 четверть_9_JavaScript_Vue.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E64927-27A1-458D-B0A7-3E2A02AD0E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45559D31-AAFB-4191-8C89-562D186D0B50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="-18840" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2790" yWindow="-17325" windowWidth="27330" windowHeight="12000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Название 1-3" sheetId="12" r:id="rId1"/>
-    <sheet name="Vue Css" sheetId="17" r:id="rId2"/>
+    <sheet name="Vue Css" sheetId="21" r:id="rId2"/>
     <sheet name="URL to login after REMOTE auth" sheetId="20" r:id="rId3"/>
     <sheet name="ElComponent" sheetId="18" r:id="rId4"/>
     <sheet name="El-dialog" sheetId="19" r:id="rId5"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="511">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -7644,43 +7644,6 @@
     <t>Результат должен быть</t>
   </si>
   <si>
-    <t>Вариант 3</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                &lt;el-button
-                   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :style="condformattingobj.colorformatting?.active ? activeStyleColor : {}"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                &gt;
-                &lt;/el-button&gt;</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">data() {
         return {
@@ -7716,21 +7679,191 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">                &lt;el-button
-                   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :style="{backgroundColor: "#409EFF",}"</t>
+    <t>inline стили</t>
+  </si>
+  <si>
+    <t>несколько стилей</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;el-button</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :style="{backgroundColor: "#409EFF", ...}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  &gt; &lt;/el-button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>несколько стилей с условиями</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;el-button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:style="{backgroundColor: item.length === 0 ? "#409EFF" : "#FFF", ...}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt; &lt;/el-button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>несколько стилей, комбинированных в объект</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;el-button</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :style="condformattingobj.colorformatting?.active ? activeStyleColor : {}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt; &lt;/el-button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>классы</t>
+  </si>
+  <si>
+    <t>Подход 1</t>
+  </si>
+  <si>
+    <t>один class</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;button  v-bind:class=" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "&gt; &lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Подход 2</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;button  v-bind:class="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{'btn-danger': !colorEdit || !baseSettings.editUserCurrentSetting}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "&gt; &lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>несколько class</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;button 
+         v-bind:class="
+        [
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null ,
+          colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null </t>
     </r>
     <r>
       <rPr>
@@ -7742,26 +7875,31 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-                &gt;
-                &lt;/el-button&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                &lt;el-button
-                   </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> :style="{backgroundColor: item.length === 0 ? "#409EFF" : "#FFF",}"</t>
+         ]
+       "
+&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;button 
+         v-bind:class="
+        {
+          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'btn-danger': colorEdit &amp;&amp; baseSettings.editUserCurrentSetting,
+          'btn-default': !colorEdit || !baseSettings.editUserCurrentSetting, 
+          'btn-primary': colorEdit &amp;&amp; !baseSettings.editUserCurrentSetting</t>
     </r>
     <r>
       <rPr>
@@ -7773,30 +7911,33 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-                &gt;
-                &lt;/el-button&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                      &lt;button 
-                              v-bind:class="
-                              {
-                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>'btn-danger': colorEdit &amp;&amp; baseSettings.editUserCurrentSetting,
-                                'btn-default': !colorEdit || !baseSettings.editUserCurrentSetting, 
-                                'btn-primary': colorEdit &amp;&amp; !baseSettings.editUserCurrentSetting</t>
+         }
+       "
+&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Микс подход</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;button 
+        v-bind:class="[
+           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">'custom_class_1',
+            {'btn-danger': !colorEdit || !baseSettings.editUserCurrentSetting}, 
+           colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null </t>
     </r>
     <r>
       <rPr>
@@ -7808,132 +7949,85 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-                              }
-                              "
-                      &lt;/button&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                      &lt;button 
-                              v-bind:class=" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "
-                      &lt;/button&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>&lt;template&gt;
-  &lt;button :class="buttonClass"&gt;Кнопка&lt;/button&gt;
+         ]"
+&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;template&gt;
+  &lt;button :class="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>buttonClass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"&gt;Кнопка&lt;/button&gt;
 &lt;/template&gt;
 &lt;script&gt;
 export default {
   computed: {
-    buttonClass() {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    buttonClass() {
       return this.checkBtn(this.table.TableNameReal) 
         ? 'btn-primary' 
         : 'hwc-btn-unactive';
     }
-  }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  }
 }
 &lt;/script&gt;</t>
-  </si>
-  <si>
-    <t>Вариант 4</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">                      &lt;button 
-                              v-bind:class="
-                              [
-                                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">'custom_class_1',
-                                {'btn-danger': !colorEdit || !baseSettings.editUserCurrentSetting}, 
-                                colorEdit &amp;&amp; baseSettings.editUserCurrentSetting ? 'btn-danger' : null </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                              ]
-                              "
-                      &lt;/button&gt;</t>
-    </r>
-  </si>
-  <si>
-    <t>когда 1 class</t>
-  </si>
-  <si>
-    <t>когда несколько class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">через computed </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="42">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -8353,12 +8447,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -8369,20 +8464,20 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -8394,7 +8489,7 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -8403,63 +8498,54 @@
     <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="19" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="14" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8467,7 +8553,7 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="35" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="33" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -8476,8 +8562,8 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="33" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8485,23 +8571,20 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8509,28 +8592,16 @@
     <xf numFmtId="49" fontId="6" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -8539,32 +8610,70 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="13" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="41" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="13" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{141A142D-D8A7-43F9-B8D2-54AA311FA1CB}"/>
+    <cellStyle name="Обычный 2 2" xfId="3" xr:uid="{C739D4B1-2A16-47B8-8914-B47AE649C078}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -12028,7 +12137,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -12036,201 +12145,203 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEF32088-FDD0-46A0-946F-1A7398394841}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A9F60E-4ADA-4D72-A128-02A784820C6B}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V12"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36" style="19" customWidth="1"/>
-    <col min="2" max="2" width="50.5546875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="85.21875" style="20" customWidth="1"/>
-    <col min="4" max="4" width="56.44140625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" style="18" customWidth="1"/>
-    <col min="6" max="6" width="43.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.109375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" style="19" customWidth="1"/>
-    <col min="9" max="9" width="64.33203125" style="19" customWidth="1"/>
-    <col min="10" max="10" width="7.77734375" style="18" customWidth="1"/>
-    <col min="11" max="11" width="39.21875" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="19" customWidth="1"/>
-    <col min="13" max="13" width="72.6640625" style="19" customWidth="1"/>
-    <col min="14" max="14" width="43.88671875" style="19" customWidth="1"/>
-    <col min="15" max="15" width="7.77734375" style="18" customWidth="1"/>
-    <col min="16" max="16" width="56.77734375" style="20" customWidth="1"/>
-    <col min="17" max="17" width="46.77734375" style="20" customWidth="1"/>
-    <col min="18" max="18" width="62.88671875" style="20" customWidth="1"/>
-    <col min="19" max="19" width="49.21875" style="19" customWidth="1"/>
-    <col min="20" max="20" width="8.77734375" style="21"/>
-    <col min="21" max="21" width="67.77734375" style="20" customWidth="1"/>
-    <col min="22" max="22" width="68.33203125" style="19" customWidth="1"/>
-    <col min="23" max="24" width="59.33203125" style="19" customWidth="1"/>
-    <col min="25" max="25" width="59.6640625" style="19" customWidth="1"/>
-    <col min="26" max="26" width="99.44140625" style="19" customWidth="1"/>
-    <col min="27" max="27" width="41.21875" style="19" customWidth="1"/>
-    <col min="28" max="16384" width="8.77734375" style="19"/>
+    <col min="1" max="1" width="36" style="66" customWidth="1"/>
+    <col min="2" max="2" width="50.5546875" style="67" customWidth="1"/>
+    <col min="3" max="3" width="100.44140625" style="67" customWidth="1"/>
+    <col min="4" max="4" width="56.44140625" style="66" customWidth="1"/>
+    <col min="5" max="5" width="6.21875" style="65" customWidth="1"/>
+    <col min="6" max="6" width="43.21875" style="66" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.109375" style="67" customWidth="1"/>
+    <col min="8" max="8" width="67.88671875" style="66" customWidth="1"/>
+    <col min="9" max="9" width="64.33203125" style="66" customWidth="1"/>
+    <col min="10" max="10" width="7.77734375" style="65" customWidth="1"/>
+    <col min="11" max="11" width="39.21875" style="66" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.88671875" style="66" customWidth="1"/>
+    <col min="13" max="13" width="72.6640625" style="66" customWidth="1"/>
+    <col min="14" max="14" width="43.88671875" style="66" customWidth="1"/>
+    <col min="15" max="15" width="7.77734375" style="65" customWidth="1"/>
+    <col min="16" max="16" width="56.77734375" style="67" customWidth="1"/>
+    <col min="17" max="17" width="46.77734375" style="67" customWidth="1"/>
+    <col min="18" max="18" width="62.88671875" style="67" customWidth="1"/>
+    <col min="19" max="19" width="49.21875" style="66" customWidth="1"/>
+    <col min="20" max="20" width="8.77734375" style="68"/>
+    <col min="21" max="21" width="67.77734375" style="67" customWidth="1"/>
+    <col min="22" max="22" width="68.33203125" style="66" customWidth="1"/>
+    <col min="23" max="24" width="59.33203125" style="66" customWidth="1"/>
+    <col min="25" max="25" width="59.6640625" style="66" customWidth="1"/>
+    <col min="26" max="26" width="99.44140625" style="66" customWidth="1"/>
+    <col min="27" max="27" width="41.21875" style="66" customWidth="1"/>
+    <col min="28" max="16384" width="8.77734375" style="66"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
-      <c r="S2" s="23"/>
-      <c r="U2" s="23"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="U2" s="70"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="71" t="s">
         <v>463</v>
       </c>
-      <c r="P3" s="19"/>
-      <c r="U3" s="19"/>
-      <c r="V3" s="20"/>
-    </row>
-    <row r="4" spans="1:22" s="18" customFormat="1">
-      <c r="A4" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="19"/>
-    </row>
-    <row r="5" spans="1:22" ht="129.6">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="P3" s="66"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="67"/>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="72" t="s">
+        <v>492</v>
+      </c>
+      <c r="P4" s="66"/>
+      <c r="U4" s="66"/>
+      <c r="V4" s="67"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="64" t="s">
         <v>493</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="73" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="57.6">
-      <c r="A6" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="64" t="s">
         <v>495</v>
       </c>
+      <c r="C6" s="73" t="s">
+        <v>496</v>
+      </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:22" ht="57.6">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:22" ht="129.6">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>498</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>496</v>
-      </c>
-      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="52" t="s">
-        <v>492</v>
+      <c r="A8" s="72" t="s">
+        <v>499</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="64"/>
+      <c r="C8" s="73"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="57.6">
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>500</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C9" s="73" t="s">
         <v>502</v>
       </c>
-      <c r="C9" s="68" t="s">
-        <v>498</v>
-      </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:22" ht="129.6">
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>503</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>504</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" ht="115.2">
+      <c r="A11" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C11" s="73" t="s">
+        <v>506</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" ht="129.6">
+      <c r="A12" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="C10" s="64" t="s">
-        <v>497</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:22" ht="129.6">
-      <c r="A11" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>501</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:22" ht="216">
-      <c r="A12" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="B12" s="67" t="s">
-        <v>504</v>
-      </c>
-      <c r="C12" s="67" t="s">
-        <v>499</v>
+      <c r="B12" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>507</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:22" ht="100.8">
+      <c r="A13" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>509</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:22" ht="216">
+      <c r="A14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -12279,10 +12390,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="22"/>
@@ -12304,7 +12415,7 @@
       <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="55" t="s">
         <v>482</v>
       </c>
       <c r="P3" s="19"/>
@@ -12312,11 +12423,11 @@
       <c r="V3" s="20"/>
     </row>
     <row r="4" spans="1:22" s="18" customFormat="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="56" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="20"/>
-      <c r="C4" s="63"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="20"/>
@@ -12335,11 +12446,11 @@
       <c r="V4" s="19"/>
     </row>
     <row r="5" spans="1:22" s="18" customFormat="1">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="60" t="s">
         <v>490</v>
       </c>
       <c r="B5" s="20"/>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="61" t="s">
         <v>489</v>
       </c>
       <c r="D5" s="19"/>
@@ -12364,7 +12475,7 @@
         <v>485</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="57" t="s">
         <v>486</v>
       </c>
       <c r="D6" s="2"/>
@@ -12374,16 +12485,16 @@
         <v>484</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="57" t="s">
         <v>483</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="409.6">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="58" t="s">
         <v>487</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C8" s="59" t="s">
         <v>488</v>
       </c>
     </row>
@@ -12443,10 +12554,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="22"/>
@@ -12468,10 +12579,10 @@
       <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="51" t="s">
         <v>465</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="52" t="s">
         <v>464</v>
       </c>
       <c r="P3" s="19"/>
@@ -12531,10 +12642,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="22"/>
@@ -12556,74 +12667,74 @@
       <c r="U2" s="23"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="51" t="s">
         <v>481</v>
       </c>
-      <c r="D3" s="54"/>
+      <c r="D3" s="52"/>
       <c r="P3" s="19"/>
       <c r="U3" s="19"/>
       <c r="V3" s="20"/>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="54" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="129.6">
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="53" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="216">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="52" t="s">
         <v>470</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="53" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="316.8">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="52" t="s">
         <v>471</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="53" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="360">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="C8" s="55" t="s">
+      <c r="C8" s="53" t="s">
         <v>473</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="331.2">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="52" t="s">
         <v>476</v>
       </c>
-      <c r="C9" s="55" t="s">
+      <c r="C9" s="53" t="s">
         <v>467</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="374.4">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="52" t="s">
         <v>475</v>
       </c>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="53" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="56" t="s">
+      <c r="A11" s="54" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="409.6">
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="53" t="s">
         <v>478</v>
       </c>
-      <c r="C12" s="55" t="s">
+      <c r="C12" s="53" t="s">
         <v>477</v>
       </c>
     </row>
@@ -12679,10 +12790,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="22"/>
@@ -12832,12 +12943,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="22"/>
@@ -12954,10 +13065,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="65"/>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="A1" s="62"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" s="22"/>

</xml_diff>